<commit_message>
Updates path list excel file
</commit_message>
<xml_diff>
--- a/files/path_list.xlsx
+++ b/files/path_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\excelsampledata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwthomson\powershell_scripts\imageresize\powershell image resize BAS\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6EC5D8-3893-42F6-BBE2-FB5A3EAF76C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CCF55E-7DD8-4C7A-A9E6-597165D7ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12636" yWindow="4608" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="204" yWindow="2964" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="include" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>path</t>
   </si>
@@ -34,9 +34,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>C:\Temp\images\</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -44,6 +41,15 @@
   </si>
   <si>
     <t>C:\Temp\images\folder2\folder2-sub2</t>
+  </si>
+  <si>
+    <t>C:\Temp\images1\</t>
+  </si>
+  <si>
+    <t>C:\Temp\images2\images2-sub2\images2-sub2-sub2\</t>
+  </si>
+  <si>
+    <t>C:\Temp\images2\images2-sub2\images2-sub2-sub2\images2-sub2-sub2-sub1</t>
   </si>
 </sst>
 </file>
@@ -361,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -375,7 +381,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -386,7 +392,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -396,10 +410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9BFF8-B01E-40C0-BF74-7EE0C47B4272}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,7 +423,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -420,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -428,7 +442,12 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed exclude path bug in path_list file
</commit_message>
<xml_diff>
--- a/files/path_list.xlsx
+++ b/files/path_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwthomson\powershell_scripts\imageresize\powershell image resize BAS\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CCF55E-7DD8-4C7A-A9E6-597165D7ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5334EC17-17A9-4417-96F9-7F477E6BE439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="2964" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="include" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>path</t>
   </si>
@@ -37,19 +37,10 @@
     <t>type</t>
   </si>
   <si>
-    <t>C:\Temp\images\folder2\folder2-sub1</t>
-  </si>
-  <si>
-    <t>C:\Temp\images\folder2\folder2-sub2</t>
-  </si>
-  <si>
     <t>C:\Temp\images1\</t>
   </si>
   <si>
-    <t>C:\Temp\images2\images2-sub2\images2-sub2-sub2\</t>
-  </si>
-  <si>
-    <t>C:\Temp\images2\images2-sub2\images2-sub2-sub2\images2-sub2-sub2-sub1</t>
+    <t>C:\Temp\images1\folder2</t>
   </si>
 </sst>
 </file>
@@ -367,19 +358,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -387,20 +378,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -410,18 +393,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9BFF8-B01E-40C0-BF74-7EE0C47B4272}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -429,25 +412,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed path in include list and changed variable name
</commit_message>
<xml_diff>
--- a/files/path_list.xlsx
+++ b/files/path_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwthomson\powershell_scripts\imageresize\powershell image resize BAS\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5334EC17-17A9-4417-96F9-7F477E6BE439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0D1D79-1EDA-4EA5-83F4-CF5FACE8BE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="include" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>path</t>
   </si>
@@ -37,10 +37,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>C:\Temp\images1\</t>
-  </si>
-  <si>
-    <t>C:\Temp\images1\folder2</t>
+    <t>C:\Temp\COW reports\</t>
   </si>
 </sst>
 </file>
@@ -360,8 +357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,10 +390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9BFF8-B01E-40C0-BF74-7EE0C47B4272}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,14 +409,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>